<commit_message>
Se corrigieron pruebas funcionales
</commit_message>
<xml_diff>
--- a/documentacion/RTM.xlsx
+++ b/documentacion/RTM.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\Servicio\SistemaGeolocalizacion\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omar_\Documents\ING SOFTWARE\LABSOL\SistemaGeolocalizacion\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C1EB92-D4C9-463D-96C6-6AB08209F249}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C335E5C-FAA9-479F-A8AA-29FF0626B60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unitarias" sheetId="1" r:id="rId1"/>
+    <sheet name="Funcionales" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="119">
   <si>
     <t>MATRIZ DE TRAZABILIDAD DE REQUERIMIENTOS</t>
   </si>
@@ -298,6 +299,111 @@
   <si>
     <t>acti</t>
   </si>
+  <si>
+    <t>ID Validación Funcional</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>F14</t>
+  </si>
+  <si>
+    <t>F15</t>
+  </si>
+  <si>
+    <t>F16</t>
+  </si>
+  <si>
+    <t>F17</t>
+  </si>
+  <si>
+    <t>F18</t>
+  </si>
+  <si>
+    <t>F19</t>
+  </si>
+  <si>
+    <t>F20</t>
+  </si>
+  <si>
+    <t>F21</t>
+  </si>
+  <si>
+    <t>F22</t>
+  </si>
+  <si>
+    <t>F23</t>
+  </si>
+  <si>
+    <t>F24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R04
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R05
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R06
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R09
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11
+</t>
+  </si>
+  <si>
+    <t>No. Escenario</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
 </sst>
 </file>
 
@@ -306,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\,\ m"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -348,6 +454,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -518,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -558,6 +669,12 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -568,10 +685,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,10 +908,10 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.25" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -804,20 +921,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -837,7 +954,7 @@
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -851,7 +968,7 @@
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -865,7 +982,7 @@
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -879,7 +996,7 @@
       <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -893,7 +1010,7 @@
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -907,7 +1024,7 @@
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -921,7 +1038,7 @@
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -935,7 +1052,7 @@
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -949,7 +1066,7 @@
       <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -963,7 +1080,7 @@
       <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -977,7 +1094,7 @@
       <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -991,7 +1108,7 @@
       <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1005,7 +1122,7 @@
       <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1019,7 +1136,7 @@
       <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1033,7 +1150,7 @@
       <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1047,7 +1164,7 @@
       <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1061,7 +1178,7 @@
       <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1075,7 +1192,7 @@
       <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1089,7 +1206,7 @@
       <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1103,7 +1220,7 @@
       <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1117,7 +1234,7 @@
       <c r="A24" s="4">
         <v>21</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -1131,7 +1248,7 @@
       <c r="A25" s="4">
         <v>22</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1145,7 +1262,7 @@
       <c r="A26" s="4">
         <v>23</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1159,7 +1276,7 @@
       <c r="A27" s="4">
         <v>24</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1173,7 +1290,7 @@
       <c r="A28" s="4">
         <v>25</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1187,7 +1304,7 @@
       <c r="A29" s="4">
         <v>26</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1201,7 +1318,7 @@
       <c r="A30" s="4">
         <v>27</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -1215,7 +1332,7 @@
       <c r="A31" s="4">
         <v>28</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1229,7 +1346,7 @@
       <c r="A32" s="4">
         <v>29</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -1243,7 +1360,7 @@
       <c r="A33" s="4">
         <v>30</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -1257,7 +1374,7 @@
       <c r="A34" s="4">
         <v>31</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1271,7 +1388,7 @@
       <c r="A35" s="4">
         <v>32</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -1285,7 +1402,7 @@
       <c r="A36" s="4">
         <v>33</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -1299,7 +1416,7 @@
       <c r="A37" s="4">
         <v>34</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -1313,7 +1430,7 @@
       <c r="A38" s="4">
         <v>35</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -1327,7 +1444,7 @@
       <c r="A39" s="4">
         <v>36</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="15" t="s">
         <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -1341,7 +1458,7 @@
       <c r="A40" s="4">
         <v>37</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="15" t="s">
         <v>51</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -1355,7 +1472,7 @@
       <c r="A41" s="4">
         <v>38</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="15" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -1369,7 +1486,7 @@
       <c r="A42" s="4">
         <v>39</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="15" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -1383,7 +1500,7 @@
       <c r="A43" s="4">
         <v>40</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -1397,7 +1514,7 @@
       <c r="A44" s="4">
         <v>41</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -1411,7 +1528,7 @@
       <c r="A45" s="4">
         <v>42</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -1425,7 +1542,7 @@
       <c r="A46" s="4">
         <v>43</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -1439,7 +1556,7 @@
       <c r="A47" s="4">
         <v>44</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="15" t="s">
         <v>63</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -1453,7 +1570,7 @@
       <c r="A48" s="4">
         <v>45</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="15" t="s">
         <v>65</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -1467,7 +1584,7 @@
       <c r="A49" s="4">
         <v>46</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -1481,7 +1598,7 @@
       <c r="A50" s="4">
         <v>47</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -1495,7 +1612,7 @@
       <c r="A51" s="4">
         <v>48</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -1509,7 +1626,7 @@
       <c r="A52" s="4">
         <v>49</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -1523,7 +1640,7 @@
       <c r="A53" s="4">
         <v>50</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -1537,7 +1654,7 @@
       <c r="A54" s="4">
         <v>51</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -1551,7 +1668,7 @@
       <c r="A55" s="4">
         <v>52</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -1565,7 +1682,7 @@
       <c r="A56" s="4">
         <v>53</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -1579,7 +1696,7 @@
       <c r="A57" s="4">
         <v>54</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -1593,7 +1710,7 @@
       <c r="A58" s="4">
         <v>55</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -1607,7 +1724,7 @@
       <c r="A59" s="4">
         <v>56</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -4970,4 +5087,396 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E721966B-3E62-406B-B833-F1BA668911AF}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>13</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>14</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>15</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>18</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>19</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>20</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>21</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>22</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>23</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>24</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="23">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>